<commit_message>
Add new routes for detalle_evidencia_vok and api_ultimo_archivo_subido; update templates for improved client filtering and detail display
</commit_message>
<xml_diff>
--- a/semana/semana_completa_14.xlsx
+++ b/semana/semana_completa_14.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28908"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E328C79-06F3-4EEE-9950-74E9ED9DE094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1640AD0-B471-4F78-A898-7A9ADFA8306D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="Detalle_VOK" sheetId="3" r:id="rId3"/>
     <sheet name="Carta_cr" sheetId="4" r:id="rId4"/>
     <sheet name="Detalle_cr" sheetId="5" r:id="rId5"/>
+    <sheet name="Evidencia_vok" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3616" uniqueCount="868">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3984" uniqueCount="952">
   <si>
     <t>c</t>
   </si>
@@ -2639,13 +2640,265 @@
   </si>
   <si>
     <t>E-WEL-N0002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLANTA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RUTAS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">V MALOS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROBLEMA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INICIA A MEDIADOS DEL PUNTO 1 Y PUNTO 2 Y NO REGISTRA EL PUNTO 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO INICIA EN EL PUNTO 1 </t>
+  </si>
+  <si>
+    <t>NO REALIZA ALTO EN EL PUTNO 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIDAD CONFIRMADA NO REALIZA RECORRDO, INICIA EN PUNTO 5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INICIA EN PUNTO 3 </t>
+  </si>
+  <si>
+    <t>UNIDAD CONFIRMADA NO REALIZA RECORRDO, INICIA EN PUNTO 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERROR DE SISTEMA NO REGISTRA PUNTO FINAL </t>
+  </si>
+  <si>
+    <t>INICIA ANTES EL RECORRIDO Y NO REGISTRA EL PUNTO 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO REGISTRA EL PUNTO 1 , INICIA EN PUNTO 6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERROR DE SISTEMA NO REGISTRA PUNTO 1, INICIA EN PUNTO 3 </t>
+  </si>
+  <si>
+    <t>INICIA ANTES EL RECORRIDO Y NO REALIZA AL TOTAL EN PUNTO 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INICIA TARDE EL RECORRIDO HE LLEGA TARDE Y NO REGISTRA LOS PUNTO 1 O FINAL , INICIA EN PUNTO 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INICIA A MEDIADO DEL RECORRIDO, NO REALIZA ALTO TOTAL EN PUNTO 1 Y PASANTO TARDE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HACE ALTO MAS ADELANTE DEL PUNTO 1 , NO REALIZA ALTO EN EL PUNTO 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIDAD CONFIRMADA NO REALIZA RECORRIDO PROGRAMADO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERROR DE SISTEMA NO REGISTRA EL PUNTO 1 </t>
+  </si>
+  <si>
+    <t>INICIA TARDE Y NO REGISTRA EL PUNTO 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO REGISTRA PUNTO FINAL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LLEGADAS TARDE A PLANTA NO REGISTRA PUNTO FINAL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LLEGADA TARDE A PLANTA NO REGISTRA PUNTO FINAL, SE VUELVE ACOMODAR PUTNO 1 YA QUE EL OPERADOR INICIO A LA REFERENCIA DEL COORDINADOR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE ACOMODA PUNTO 1 YA QUE NO REGISTRABA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIDAD PROGRAMADA NO REALIZA RECORRIDO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO REALIZA ALTO EN EL PUNTO 1 Y UNIDAD CONFIRMADA NO REALIZA RECORRIDO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO REALIZA ALTO EN EL PUTNO 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO REGISRA EL PUNTO FINAL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INICIA EN PUNTO 3, EL PUNTO FINAL DE ACOMODA YA QUE NO ESTA HACIENDO ALTO Y SE ACOMODA POR ORDEN DEL COORDINADOR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIDAD PROGRAMADA NO REALIZA RECORRIDO, SE ACOMODA PUNTO YA QUE NO REALIZA ALTO DONDE INDICO COORDINADOR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VARIA EL ALTO DEL PUNTO 1 Y NO LO REGISTRA  Y NO REALIA ALTO EN PUNTO FINAL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO REALIZA ALTO EN PUNTO 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INICIA EN UN PUNTO DIFERENTE DE LA REFERENCIA DEL PUNTO 1 </t>
+  </si>
+  <si>
+    <t>NO INICIA EN PUNTO 1, INICIA ANTES EL RECORRIDO Y NO REGISTRA EL PUNTO 1</t>
+  </si>
+  <si>
+    <t>NO REALIZA ALTO TOTAL EN PUNTO 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INICIA TARDE Y NO REGISTRA EL PUNTO 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INICIA TARDE EL RECORRIDO Y NO REGISTRA PUNTO 1, ERROR DE SISTEMA NO REGISTRA PUNTO 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INICIA TARDE EL RECORRIDO Y NO REGISTRA PUNTO 1 </t>
+  </si>
+  <si>
+    <t>INICIA ANTES Y NO REGISTRA PUNTO 1, INICIA TARDE Y NO REALIZA ALTO EN PUNTO 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INICIA TARDE EL RECORRIDO Y NO REGISTRA EL PUNTO 1, INICIA A MEDIADOS DEL RECORRIDO </t>
+  </si>
+  <si>
+    <t>INICIA TARDEO O INICIA ANTES  EL RECORRIDO Y NO REGISTRA EL PUNTO 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO REGISTRA EL PUNTO FINAL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERROR DE SISTEMA NO REGISTRA EL PUNTO FINAL Y LLEGADA TARDE NO REGISTRA EL PUNTO FINAL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERROR DE SISTEMA NO REGISTRA PUNTO 1 </t>
+  </si>
+  <si>
+    <t>NO REALIZA ALTO TOTAL EN PUNTO 1, INICIA TARDE Y NO REGISTRA EL PUNTO 1 Y ERROR DE SISTEMA NO REGISTRA PUNTO 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INICIA TARDE EL RECORRIDO, INICIA A MEDIADOS DEL RECORRIDO, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INICIA A MEDIADOS DEL RECORRIDO, NO REALIZA ALTO TOTAL EN PUTNO 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INICIA A MEDIADOS DEL RECORRIDO, INIICA EN OTRO LADO DEL PUNTO 1 INICIANDO ANTES Y NO REGISTRA PUNTO 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INICIA A MEDIADOS DEL RECORRIDO, NO PASA POR EL PUNTO 1 HE INICIA TARDE EL RECORRIDO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INICIA ANTES EL RECORRIDO Y NO REGISTRA EL PUNTO 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE SALTA LOS PRIMERO PUNTOS INICIANDO EN PUNTO 5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INICIA ANTES EL RECORRIDO Y NO REALIZANDO ALTO TOTAL EN PUNTO 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INICIA ANTES EL RECORRIDO Y NO REALIZA ALTO EN PUNTO 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INICIA ANTES EL RECORRIDO Y NO REGISTRA PUNTO 1, INICIA A MEDIADOS DEL RECORRIDO </t>
+  </si>
+  <si>
+    <t>NO REALIZA ALTO TOTAL EN PUNTO 1, INICIA EL RECORRIDO MAS ADELANTE DE LA REFERENCIA Y NO REGISTRA PUNTO 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERRRO DE COORDENADAS DE GPS NO REGISTRA PUNTO 1 </t>
+  </si>
+  <si>
+    <t>UNIDAD CONFIRMADA NO REALIZA RECORRDO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE REALIZA CAMBIOS DE HORARIOS Y COMODO DE PUNTO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INICIA A MEDIADOS DEL RECORRIDO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INICIA TARDE EL RECORRIDO Y NO REGISTRA EL PUNTO 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIDAD CONFIRMADA NO REALIZA RECORRIDO, UNIDAD LLEGA TARDE A PLANTA Y NO REGISTRA PUNTO FINAL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INICIA EN PUNTO 2 HE INICIA TARDE EL RECORRIDO Y NO REIGSTRA PUNTO 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INICIA EN EL PUNTO 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO PASA POR EL PUNTO 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TURNO 1 INICIA 10 MINUTOS ANTES Y NO REGISTRA PUNTO 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INICIA ANTES EL RECORRIDO, INICIA A MEDIADOS DEL RECORRIDO </t>
+  </si>
+  <si>
+    <t>REALIZA ALTO MAS ADELANTE DEL PUNTO DE REFERENCIA Y NO REGISTRA EL PUNTO 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INICIA ANTES EL RECORRIDO Y NO REGISTRA PUNTO 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPERADOR QUE INTENTE INICIAR EN EL MISMO PUNTO PARA QUE REGISTRE EL PUNTO 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INICIA TARDE EL RECORRIDO Y NO REALIZA ALTO TOTAL EN PUNTO 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERROR DE SISTEMA NO REGISTRA PUNTO FINAL, INICIA ANTES O NO PASA POR EL PUNTO 1 POR LO CUAL NO LO REGISTRA PUNTO 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO PASA POR EL PUNTO 1 Y NO LO REGISTRA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO REALIZA ALTO EN PUNTO 1 HE INICIA A MEDIADOS DEL RECORRIDO </t>
+  </si>
+  <si>
+    <t>NO REALIZA ALTO TOTAL HE INICIA ANTES EL RECORRIDO Y NO REGISTRA PUNTO 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INICIA ANTES EL RECORRIDO Y NO REGISTRA PUNTO 1, UNIDAD CONFIRMADA NO REALIZA RECORRIDO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIDAD CONFIRMADA NO REALIZA RECORRIDO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERROR DE SISTEMA NO REGISTRA EL PUNTO 1 Y FINAL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INICIA ANTES EL RECORRIDO Y NO REALIZA ALTO TOTAL EN PUNTO 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO REALIZA ALTO EN PUNTO 1 HE INICIA EN PUNTO 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INICIA A MEDIACION DEL RECORRIDO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INICIA A MEDIADOS DEL RECORRIDO, ERROR DE SISTEMA NO REGISTRA PUNTO FINAL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INICIA ANTES EL RECORRIDO, ERROR DE SISTEMA NO REGISTRA EN PUNTO 1, NO PASA POR EL PUNTO 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INICIA EN PUNTO 2, INICIA TARDE EL RECORRIDO Y NO REGISTRA PUNTO 1 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2658,16 +2911,55 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB5E6A2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7E36F"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -2690,17 +2982,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -30741,7 +31070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2124BDFF-B84E-43A9-A73E-8BED6BD7273B}">
   <dimension ref="A1:F371"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C45" sqref="A45:C45"/>
     </sheetView>
   </sheetViews>
@@ -39704,4 +40033,1790 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE96D43C-32F1-403D-9561-8870E4EEAF60}">
+  <dimension ref="A1:D131"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D131"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="143.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="4" t="s">
+        <v>868</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>869</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C2" s="9">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C3" s="9">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>203</v>
+      </c>
+      <c r="C4" s="9">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>233</v>
+      </c>
+      <c r="C5" s="9">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>250</v>
+      </c>
+      <c r="C6" s="9">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C7" s="9">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>228</v>
+      </c>
+      <c r="C8" s="9">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C9" s="9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>238</v>
+      </c>
+      <c r="C10" s="9">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>223</v>
+      </c>
+      <c r="C11" s="9">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>333</v>
+      </c>
+      <c r="C12" s="9">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="9">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>238</v>
+      </c>
+      <c r="C14" s="9">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="9">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>205</v>
+      </c>
+      <c r="C16" s="9">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="9">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>204</v>
+      </c>
+      <c r="C18" s="9">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>197</v>
+      </c>
+      <c r="C19" s="9">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>234</v>
+      </c>
+      <c r="C20" s="9">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" t="s">
+        <v>415</v>
+      </c>
+      <c r="C21" s="9">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>283</v>
+      </c>
+      <c r="C22" s="9">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" t="s">
+        <v>407</v>
+      </c>
+      <c r="C23" s="9">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" t="s">
+        <v>397</v>
+      </c>
+      <c r="C24" s="9">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" t="s">
+        <v>403</v>
+      </c>
+      <c r="C25" s="9">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" t="s">
+        <v>396</v>
+      </c>
+      <c r="C26" s="9">
+        <v>3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" t="s">
+        <v>399</v>
+      </c>
+      <c r="C27" s="9">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" t="s">
+        <v>340</v>
+      </c>
+      <c r="C28" s="9">
+        <v>3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" t="s">
+        <v>234</v>
+      </c>
+      <c r="C29" s="9">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" t="s">
+        <v>394</v>
+      </c>
+      <c r="C30" s="9">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" t="s">
+        <v>421</v>
+      </c>
+      <c r="C31" s="9">
+        <v>2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="9">
+        <v>3</v>
+      </c>
+      <c r="D32" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" t="s">
+        <v>213</v>
+      </c>
+      <c r="C33" s="9">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" t="s">
+        <v>212</v>
+      </c>
+      <c r="C34" s="9">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" t="s">
+        <v>162</v>
+      </c>
+      <c r="C35" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" t="s">
+        <v>291</v>
+      </c>
+      <c r="C36" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" t="s">
+        <v>289</v>
+      </c>
+      <c r="C37" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" t="s">
+        <v>290</v>
+      </c>
+      <c r="C38" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39" t="s">
+        <v>241</v>
+      </c>
+      <c r="C39" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" t="s">
+        <v>244</v>
+      </c>
+      <c r="C40" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" t="s">
+        <v>220</v>
+      </c>
+      <c r="C41" s="9">
+        <v>4</v>
+      </c>
+      <c r="D41" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" t="s">
+        <v>212</v>
+      </c>
+      <c r="C42" s="9">
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" t="s">
+        <v>214</v>
+      </c>
+      <c r="C43" s="9">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B44" t="s">
+        <v>279</v>
+      </c>
+      <c r="C44" s="9">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B45" t="s">
+        <v>276</v>
+      </c>
+      <c r="C45" s="9">
+        <v>1</v>
+      </c>
+      <c r="D45" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B46" t="s">
+        <v>71</v>
+      </c>
+      <c r="C46" s="9">
+        <v>12</v>
+      </c>
+      <c r="D46" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" s="9">
+        <v>5</v>
+      </c>
+      <c r="D47" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B48" t="s">
+        <v>72</v>
+      </c>
+      <c r="C48" s="9">
+        <v>4</v>
+      </c>
+      <c r="D48" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B49" t="s">
+        <v>59</v>
+      </c>
+      <c r="C49" s="9">
+        <v>3</v>
+      </c>
+      <c r="D49" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B50" t="s">
+        <v>60</v>
+      </c>
+      <c r="C50" s="9">
+        <v>3</v>
+      </c>
+      <c r="D50" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B51" t="s">
+        <v>66</v>
+      </c>
+      <c r="C51" s="9">
+        <v>3</v>
+      </c>
+      <c r="D51" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B52" t="s">
+        <v>67</v>
+      </c>
+      <c r="C52" s="9">
+        <v>3</v>
+      </c>
+      <c r="D52" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B53" t="s">
+        <v>301</v>
+      </c>
+      <c r="C53" s="9">
+        <v>11</v>
+      </c>
+      <c r="D53" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B54" t="s">
+        <v>66</v>
+      </c>
+      <c r="C54" s="9">
+        <v>7</v>
+      </c>
+      <c r="D54" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B55" t="s">
+        <v>56</v>
+      </c>
+      <c r="C55" s="9">
+        <v>3</v>
+      </c>
+      <c r="D55" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B56" t="s">
+        <v>63</v>
+      </c>
+      <c r="C56" s="9">
+        <v>3</v>
+      </c>
+      <c r="D56" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B57" t="s">
+        <v>241</v>
+      </c>
+      <c r="C57" s="9">
+        <v>5</v>
+      </c>
+      <c r="D57" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B58" t="s">
+        <v>59</v>
+      </c>
+      <c r="C58" s="9">
+        <v>4</v>
+      </c>
+      <c r="D58" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B59" t="s">
+        <v>373</v>
+      </c>
+      <c r="C59" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B60" t="s">
+        <v>364</v>
+      </c>
+      <c r="C60" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B61" t="s">
+        <v>379</v>
+      </c>
+      <c r="C61" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B62" t="s">
+        <v>196</v>
+      </c>
+      <c r="C62" s="9">
+        <v>17</v>
+      </c>
+      <c r="D62" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B63" t="s">
+        <v>197</v>
+      </c>
+      <c r="C63" s="9">
+        <v>10</v>
+      </c>
+      <c r="D63" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B64" t="s">
+        <v>59</v>
+      </c>
+      <c r="C64" s="9">
+        <v>4</v>
+      </c>
+      <c r="D64" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B65" t="s">
+        <v>323</v>
+      </c>
+      <c r="C65" s="9">
+        <v>5</v>
+      </c>
+      <c r="D65" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B66" t="s">
+        <v>292</v>
+      </c>
+      <c r="C66" s="9">
+        <v>4</v>
+      </c>
+      <c r="D66" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B67" t="s">
+        <v>257</v>
+      </c>
+      <c r="C67" s="9">
+        <v>4</v>
+      </c>
+      <c r="D67" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B68" t="s">
+        <v>278</v>
+      </c>
+      <c r="C68" s="9">
+        <v>2</v>
+      </c>
+      <c r="D68" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B69" t="s">
+        <v>318</v>
+      </c>
+      <c r="C69" s="9">
+        <v>2</v>
+      </c>
+      <c r="D69" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B70" t="s">
+        <v>320</v>
+      </c>
+      <c r="C70" s="9">
+        <v>2</v>
+      </c>
+      <c r="D70" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B71" t="s">
+        <v>327</v>
+      </c>
+      <c r="C71" s="9">
+        <v>2</v>
+      </c>
+      <c r="D71" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B72" t="s">
+        <v>304</v>
+      </c>
+      <c r="C72" s="9">
+        <v>1</v>
+      </c>
+      <c r="D72" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B73" t="s">
+        <v>268</v>
+      </c>
+      <c r="C73" s="9">
+        <v>13</v>
+      </c>
+      <c r="D73" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B74" t="s">
+        <v>246</v>
+      </c>
+      <c r="C74" s="9">
+        <v>11</v>
+      </c>
+      <c r="D74" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B75" t="s">
+        <v>263</v>
+      </c>
+      <c r="C75" s="9">
+        <v>4</v>
+      </c>
+      <c r="D75" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B76" t="s">
+        <v>264</v>
+      </c>
+      <c r="C76" s="9">
+        <v>3</v>
+      </c>
+      <c r="D76" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B77" t="s">
+        <v>275</v>
+      </c>
+      <c r="C77" s="9">
+        <v>2</v>
+      </c>
+      <c r="D77" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B78" t="s">
+        <v>256</v>
+      </c>
+      <c r="C78" s="9">
+        <v>12</v>
+      </c>
+      <c r="D78" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B79" t="s">
+        <v>297</v>
+      </c>
+      <c r="C79" s="9">
+        <v>7</v>
+      </c>
+      <c r="D79" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B80" t="s">
+        <v>298</v>
+      </c>
+      <c r="C80" s="9">
+        <v>7</v>
+      </c>
+      <c r="D80" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B81" t="s">
+        <v>299</v>
+      </c>
+      <c r="C81" s="9">
+        <v>6</v>
+      </c>
+      <c r="D81" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B82" t="s">
+        <v>246</v>
+      </c>
+      <c r="C82" s="9">
+        <v>3</v>
+      </c>
+      <c r="D82" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B83" t="s">
+        <v>255</v>
+      </c>
+      <c r="C83" s="9">
+        <v>6</v>
+      </c>
+      <c r="D83" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B84" t="s">
+        <v>253</v>
+      </c>
+      <c r="C84" s="9">
+        <v>3</v>
+      </c>
+      <c r="D84" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B85" t="s">
+        <v>202</v>
+      </c>
+      <c r="C85" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B86" t="s">
+        <v>71</v>
+      </c>
+      <c r="C86" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B87" t="s">
+        <v>198</v>
+      </c>
+      <c r="C87" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B88" t="s">
+        <v>67</v>
+      </c>
+      <c r="C88" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B89" t="s">
+        <v>201</v>
+      </c>
+      <c r="C89" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B90" t="s">
+        <v>294</v>
+      </c>
+      <c r="C90" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B91" t="s">
+        <v>278</v>
+      </c>
+      <c r="C91" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B92" t="s">
+        <v>238</v>
+      </c>
+      <c r="C92" s="9">
+        <v>6</v>
+      </c>
+      <c r="D92" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B93" t="s">
+        <v>160</v>
+      </c>
+      <c r="C93" s="9">
+        <v>14</v>
+      </c>
+      <c r="D93" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B94" t="s">
+        <v>164</v>
+      </c>
+      <c r="C94" s="9">
+        <v>4</v>
+      </c>
+      <c r="D94" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B95" t="s">
+        <v>165</v>
+      </c>
+      <c r="C95" s="9">
+        <v>4</v>
+      </c>
+      <c r="D95" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B96" t="s">
+        <v>167</v>
+      </c>
+      <c r="C96" s="9">
+        <v>4</v>
+      </c>
+      <c r="D96" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B97" t="s">
+        <v>166</v>
+      </c>
+      <c r="C97" s="9">
+        <v>3</v>
+      </c>
+      <c r="D97" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B98" t="s">
+        <v>59</v>
+      </c>
+      <c r="C98" s="9">
+        <v>3</v>
+      </c>
+      <c r="D98" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B99" t="s">
+        <v>337</v>
+      </c>
+      <c r="C99" s="9">
+        <v>1</v>
+      </c>
+      <c r="D99" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B100" t="s">
+        <v>84</v>
+      </c>
+      <c r="C100" s="9">
+        <v>9</v>
+      </c>
+      <c r="D100" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B101" t="s">
+        <v>129</v>
+      </c>
+      <c r="C101" s="9">
+        <v>5</v>
+      </c>
+      <c r="D101" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B102" t="s">
+        <v>85</v>
+      </c>
+      <c r="C102" s="9">
+        <v>3</v>
+      </c>
+      <c r="D102" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B103" t="s">
+        <v>93</v>
+      </c>
+      <c r="C103" s="9">
+        <v>3</v>
+      </c>
+      <c r="D103" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B104" t="s">
+        <v>126</v>
+      </c>
+      <c r="C104" s="9">
+        <v>3</v>
+      </c>
+      <c r="D104" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B105" t="s">
+        <v>150</v>
+      </c>
+      <c r="C105" s="9">
+        <v>3</v>
+      </c>
+      <c r="D105" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B106" t="s">
+        <v>132</v>
+      </c>
+      <c r="C106" s="9">
+        <v>3</v>
+      </c>
+      <c r="D106" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B107" t="s">
+        <v>82</v>
+      </c>
+      <c r="C107" s="9">
+        <v>2</v>
+      </c>
+      <c r="D107" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B108" t="s">
+        <v>63</v>
+      </c>
+      <c r="C108" s="9">
+        <v>2</v>
+      </c>
+      <c r="D108" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B109" t="s">
+        <v>101</v>
+      </c>
+      <c r="C109" s="9">
+        <v>2</v>
+      </c>
+      <c r="D109" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B110" t="s">
+        <v>120</v>
+      </c>
+      <c r="C110" s="9">
+        <v>2</v>
+      </c>
+      <c r="D110" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B111" t="s">
+        <v>130</v>
+      </c>
+      <c r="C111" s="9">
+        <v>2</v>
+      </c>
+      <c r="D111" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B112" t="s">
+        <v>134</v>
+      </c>
+      <c r="C112" s="9">
+        <v>2</v>
+      </c>
+      <c r="D112" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B113" t="s">
+        <v>141</v>
+      </c>
+      <c r="C113" s="9">
+        <v>2</v>
+      </c>
+      <c r="D113" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B114" t="s">
+        <v>387</v>
+      </c>
+      <c r="C114" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B115" t="s">
+        <v>386</v>
+      </c>
+      <c r="C115" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B116" t="s">
+        <v>253</v>
+      </c>
+      <c r="C116" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B117" t="s">
+        <v>353</v>
+      </c>
+      <c r="C117" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B118" t="s">
+        <v>352</v>
+      </c>
+      <c r="C118" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B119" t="s">
+        <v>356</v>
+      </c>
+      <c r="C119" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B120" t="s">
+        <v>357</v>
+      </c>
+      <c r="C120" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B121" t="s">
+        <v>354</v>
+      </c>
+      <c r="C121" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B122" t="s">
+        <v>363</v>
+      </c>
+      <c r="C122" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B123" t="s">
+        <v>362</v>
+      </c>
+      <c r="C123" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B124" t="s">
+        <v>59</v>
+      </c>
+      <c r="C124" s="9">
+        <v>4</v>
+      </c>
+      <c r="D124" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B125" t="s">
+        <v>178</v>
+      </c>
+      <c r="C125" s="9">
+        <v>3</v>
+      </c>
+      <c r="D125" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B126" t="s">
+        <v>185</v>
+      </c>
+      <c r="C126" s="9">
+        <v>3</v>
+      </c>
+      <c r="D126" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B127" t="s">
+        <v>191</v>
+      </c>
+      <c r="C127" s="9">
+        <v>3</v>
+      </c>
+      <c r="D127" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B128" t="s">
+        <v>195</v>
+      </c>
+      <c r="C128" s="9">
+        <v>2</v>
+      </c>
+      <c r="D128" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B129" t="s">
+        <v>84</v>
+      </c>
+      <c r="C129" s="9">
+        <v>4</v>
+      </c>
+      <c r="D129" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B130" t="s">
+        <v>158</v>
+      </c>
+      <c r="C130" s="9">
+        <v>3</v>
+      </c>
+      <c r="D130" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B131" t="s">
+        <v>156</v>
+      </c>
+      <c r="C131" s="9">
+        <v>1</v>
+      </c>
+      <c r="D131" t="s">
+        <v>932</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C2:C131">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>